<commit_message>
Updated test case results.
</commit_message>
<xml_diff>
--- a/AdactInDemoProject/src/test/resources/TestData/AdactIn_TestData.xlsx
+++ b/AdactInDemoProject/src/test/resources/TestData/AdactIn_TestData.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prasha\git\adactin-hybrid-framework\AdactInDemoProject\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prasha\git\adactin\adactin_automation_framework\AdactInDemoProject\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD89C6B-221A-46A3-8A69-8D037315372C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4691BEB-6AFA-45F0-A9D2-EFEA8850CF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="6" r:id="rId1"/>
     <sheet name="Credentials" sheetId="4" r:id="rId2"/>
     <sheet name="TestCases" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$1:$H$18</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="217">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -120,9 +123,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Invalid Login details or Your Password might have expired.</t>
   </si>
   <si>
     <t>Verify successful login with valid credentials.</t>
@@ -323,9 +323,6 @@
 6. Click the "Book Now" button.</t>
   </si>
   <si>
-    <t>The booking should be removed removed.</t>
-  </si>
-  <si>
     <t>04/01/2022</t>
   </si>
   <si>
@@ -349,10 +346,6 @@
   <si>
     <t>User should not be logged in. 
 Page Title: Adactin.com - Hotel Reservation System</t>
-  </si>
-  <si>
-    <t>User redirected to "Search Hotel" page. 
-Page Title: "Adactin.com - Search Hotel".</t>
   </si>
   <si>
     <t>The user should get the hotel list/details, 
@@ -499,9 +492,6 @@
   </si>
   <si>
     <t>TC_05_Search_Hotel_WithoutLocation</t>
-  </si>
-  <si>
-    <t>"</t>
   </si>
   <si>
     <t>TC_08_Book_Hotel_MissingFirstName</t>
@@ -714,6 +704,79 @@
   </si>
   <si>
     <t>643</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>User should redirected to "Search Hotel" page. 
+Page Title: "Adactin.com - Search Hotel".</t>
+  </si>
+  <si>
+    <t>Login successful and redirected to "Search Hotel" page. 
+Page Title: "Adactin.com - Search Hotel".</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: "Enter Username".
+Page Title remained: Adactin.com - Hotel Reservation System</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: "Invalid Login details or Your Password might have expired. Click here to reset your password".
+Page Title remained: Adactin.com - Hotel Reservation System</t>
+  </si>
+  <si>
+    <t>The user got the hotel list/details, 
+Page title should be 'Select Hotel - Adactin.com'.</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: "Please Select a Location"</t>
+  </si>
+  <si>
+    <t>Expected error message as below but the system accepted backdated dates.
+- "Check-In Date shall be after today’s date."
+- "Check-Out Date shall be after Check-In Date."</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>The hotel should be successfully booked, and the user should be navigated to the Booking Confirmation page displaying the Order Number and booking details.</t>
+  </si>
+  <si>
+    <t>The hotel was successfully booked. The Booking Confirmation page was displayed with the Order Number and booking details.</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: Please Enter your First Name</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: Please Enter you Last Name</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: Please Enter your Address</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: Please Enter your 16 Digit Credit Card Number</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: Please Select your Credit Card Type</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: Please Select your Credit Card Expiry Month</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: Please Select your Credit Card Expiry Year</t>
+  </si>
+  <si>
+    <t>Expected error message displayed: Please Enter your Credit Card CVV Number</t>
+  </si>
+  <si>
+    <t>Validation failed! Expected: Hotel Creek, Sydney, Standard but got: Hotel Creek, Sydney, Deluxe</t>
+  </si>
+  <si>
+    <t>The booking should be removed.</t>
+  </si>
+  <si>
+    <t>The booking was removed as expected.</t>
   </si>
 </sst>
 </file>
@@ -799,7 +862,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -831,9 +894,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -841,12 +901,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{40B51B64-6E80-475F-89CF-F2C7E2672648}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1124,7 +1245,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC6EEC9-4E88-4AA7-B633-FDBE40A79E61}">
   <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1154,13 +1277,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>8</v>
@@ -1169,10 +1292,10 @@
         <v>9</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>10</v>
@@ -1181,63 +1304,63 @@
         <v>11</v>
       </c>
       <c r="K1" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="P1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="O1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="R1" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="S1" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
@@ -1248,39 +1371,39 @@
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
@@ -1291,39 +1414,39 @@
       <c r="Q3" s="9"/>
       <c r="R3" s="9"/>
       <c r="S3" s="9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -1334,15 +1457,15 @@
       <c r="Q4" s="9"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>2</v>
@@ -1354,19 +1477,19 @@
         <v>7</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -1377,15 +1500,15 @@
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>5</v>
@@ -1397,19 +1520,19 @@
         <v>12</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>64</v>
+        <v>53</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -1420,15 +1543,15 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>13</v>
@@ -1440,19 +1563,19 @@
         <v>4</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>65</v>
+        <v>54</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -1463,15 +1586,15 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>15</v>
@@ -1483,19 +1606,19 @@
         <v>17</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -1506,15 +1629,15 @@
       <c r="Q8" s="9"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>18</v>
@@ -1526,19 +1649,19 @@
         <v>7</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -1549,15 +1672,15 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>19</v>
@@ -1569,19 +1692,19 @@
         <v>12</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
@@ -1592,15 +1715,15 @@
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>20</v>
@@ -1612,19 +1735,19 @@
         <v>4</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>69</v>
+        <v>58</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>68</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
@@ -1635,15 +1758,15 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>21</v>
@@ -1655,19 +1778,19 @@
         <v>17</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
@@ -1678,15 +1801,15 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
       <c r="S12" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1705,15 +1828,15 @@
       <c r="Q13" s="9"/>
       <c r="R13" s="9"/>
       <c r="S13" s="9" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>15</v>
@@ -1725,19 +1848,19 @@
         <v>17</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>87</v>
+        <v>55</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
@@ -1748,15 +1871,15 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>21</v>
@@ -1768,52 +1891,52 @@
         <v>17</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="I15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K15" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="O15" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="P15" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R15" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="M15" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="N15" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="O15" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="P15" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q15" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R15" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="S15" s="13"/>
+      <c r="S15" s="12"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>15</v>
@@ -1825,52 +1948,52 @@
         <v>17</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N16" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N16" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="O16" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="O16" s="9" t="s">
+      <c r="P16" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="Q16" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q16" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>133</v>
+      <c r="R16" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>15</v>
@@ -1882,52 +2005,52 @@
         <v>17</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N17" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N17" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="O17" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="O17" s="9" t="s">
+      <c r="P17" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P17" s="9" t="s">
+      <c r="Q17" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q17" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>133</v>
+      <c r="R17" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>15</v>
@@ -1939,52 +2062,52 @@
         <v>17</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M18" s="9"/>
-      <c r="N18" s="12" t="s">
+      <c r="N18" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="O18" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="O18" s="9" t="s">
+      <c r="P18" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P18" s="9" t="s">
+      <c r="Q18" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q18" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R18" s="12" t="s">
-        <v>133</v>
+      <c r="R18" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="S18" s="7" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>15</v>
@@ -1996,52 +2119,52 @@
         <v>17</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N19" s="12"/>
+        <v>114</v>
+      </c>
+      <c r="N19" s="11"/>
       <c r="O19" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="P19" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P19" s="9" t="s">
+      <c r="Q19" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q19" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R19" s="12" t="s">
-        <v>133</v>
+      <c r="R19" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>15</v>
@@ -2053,52 +2176,52 @@
         <v>17</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N20" s="12" t="s">
-        <v>123</v>
+        <v>114</v>
+      </c>
+      <c r="N20" s="11" t="s">
+        <v>120</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q20" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q20" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R20" s="12" t="s">
-        <v>133</v>
+      <c r="R20" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="S20" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>15</v>
@@ -2110,52 +2233,52 @@
         <v>17</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K21" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="O21" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="O21" s="9" t="s">
-        <v>126</v>
-      </c>
       <c r="P21" s="9"/>
-      <c r="Q21" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R21" s="12" t="s">
-        <v>133</v>
+      <c r="Q21" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R21" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>15</v>
@@ -2167,52 +2290,52 @@
         <v>17</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N22" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N22" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="O22" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="O22" s="9" t="s">
+      <c r="P22" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P22" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q22" s="12"/>
-      <c r="R22" s="12" t="s">
-        <v>133</v>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>15</v>
@@ -2224,52 +2347,52 @@
         <v>17</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>66</v>
+        <v>55</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="N23" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N23" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="O23" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="O23" s="9" t="s">
+      <c r="P23" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="Q23" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="Q23" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R23" s="12"/>
+      <c r="R23" s="11"/>
       <c r="S23" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>2</v>
@@ -2281,52 +2404,52 @@
         <v>7</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K24" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="N24" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="N24" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="O24" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="O24" s="9" t="s">
+      <c r="P24" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="P24" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q24" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R24" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="S24" s="13"/>
+      <c r="Q24" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S24" s="12"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>19</v>
@@ -2338,52 +2461,52 @@
         <v>12</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="N25" s="12" t="s">
-        <v>187</v>
+        <v>182</v>
+      </c>
+      <c r="N25" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="P25" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q25" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R25" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="S25" s="13"/>
+        <v>127</v>
+      </c>
+      <c r="Q25" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="S25" s="12"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>20</v>
@@ -2395,52 +2518,52 @@
         <v>4</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="N26" s="12" t="s">
-        <v>191</v>
+        <v>186</v>
+      </c>
+      <c r="N26" s="11" t="s">
+        <v>187</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q26" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R26" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="S26" s="13"/>
+        <v>127</v>
+      </c>
+      <c r="Q26" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R26" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="S26" s="12"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>21</v>
@@ -2452,52 +2575,52 @@
         <v>17</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="M27" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q27" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R27" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="N27" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="O27" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="P27" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q27" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="R27" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="S27" s="13"/>
+      <c r="S27" s="12"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>5</v>
@@ -2509,45 +2632,45 @@
         <v>12</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>64</v>
+        <v>53</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M28" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="N28" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="N28" s="12" t="s">
+      <c r="O28" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="O28" s="9" t="s">
+      <c r="P28" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="P28" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q28" s="12" t="s">
+      <c r="Q28" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="R28" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="R28" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="S28" s="13"/>
+      <c r="S28" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2571,18 +2694,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>112</v>
+      <c r="A2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2594,9 +2717,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2606,8 +2729,8 @@
     <col min="3" max="3" width="41.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.88671875" style="2"/>
     <col min="10" max="10" width="49.44140625" style="2" bestFit="1" customWidth="1"/>
@@ -2616,7 +2739,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -2639,385 +2762,471 @@
       <c r="H1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="D3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="F4" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="F5" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="C6" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="D8" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="14" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="15" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="16" spans="1:10" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="144" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="D18" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>195</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="H2:H18">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",H2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",H2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H7:H8">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",H7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",H7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",H7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>